<commit_message>
first set of TestCases
</commit_message>
<xml_diff>
--- a/FreshGrocer/src/main/resources/TestData/locators.xlsx
+++ b/FreshGrocer/src/main/resources/TestData/locators.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJAY\workspace\FreshGrocer\src\main\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJAY\git\Fresh-Grocer\FreshGrocer\src\main\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC838398-8FBF-4357-997B-2E641C9298B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4485FDD-BB49-4BE9-B742-AAC1C7D9BFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="landing_page" sheetId="1" r:id="rId1"/>
-    <sheet name="login_page" sheetId="2" r:id="rId2"/>
+    <sheet name="login_page" sheetId="2" r:id="rId1"/>
+    <sheet name="landing_page" sheetId="1" r:id="rId2"/>
+    <sheet name="digital_coupons_page" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="79">
   <si>
     <t>locators name</t>
   </si>
@@ -173,6 +174,96 @@
   </si>
   <si>
     <t>.//p[contains(@class,'coupon-brand-name')]</t>
+  </si>
+  <si>
+    <t>categoriesList</t>
+  </si>
+  <si>
+    <t>signOutBtn</t>
+  </si>
+  <si>
+    <t>main-signOutLink</t>
+  </si>
+  <si>
+    <t>.//p[contains(@class,'coupon-expiration-text')]</t>
+  </si>
+  <si>
+    <t>couponDiscount</t>
+  </si>
+  <si>
+    <t>.//div[contains(@class,'coupon-value')]/p</t>
+  </si>
+  <si>
+    <t>//a[contains(text(),'Clipped') and contains(@class,'facetLink')]</t>
+  </si>
+  <si>
+    <t>clippedLink</t>
+  </si>
+  <si>
+    <t>couponExpiryDate</t>
+  </si>
+  <si>
+    <t>couponDescription</t>
+  </si>
+  <si>
+    <t>.//p[contains(@class,'coupon-desc')]</t>
+  </si>
+  <si>
+    <t>//button[contains(@class,'print-coupons-btn') and contains(text(),'Print Clipped Coupons')]</t>
+  </si>
+  <si>
+    <t>printClippedCouponBtn</t>
+  </si>
+  <si>
+    <t>clippedCouponName</t>
+  </si>
+  <si>
+    <t>//*[contains(@class,'card-body')]//h5</t>
+  </si>
+  <si>
+    <t>showImages</t>
+  </si>
+  <si>
+    <t>showImgesCheckBox</t>
+  </si>
+  <si>
+    <t>//*[contains(@class,'card-body')]//img[contains(@class,'coupon-image')]</t>
+  </si>
+  <si>
+    <t>clippedCouponImg</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'card-body')]//div[contains(@class,'value')]</t>
+  </si>
+  <si>
+    <t>clippedCouponDiscount</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'card-body')]//p[contains(@class,'expires')]</t>
+  </si>
+  <si>
+    <t>clippedCouponExpiryDate</t>
+  </si>
+  <si>
+    <t>//button[contains(text(),'Close')]</t>
+  </si>
+  <si>
+    <t>closeInPrintClippedCouponBtn</t>
+  </si>
+  <si>
+    <t>//a[contains(text(),'All Coupons') and contains(@class,'facetLink')]</t>
+  </si>
+  <si>
+    <t>//*[@title='Category']//ul/li/label</t>
+  </si>
+  <si>
+    <t>brandsList</t>
+  </si>
+  <si>
+    <t>//*[@title='Brand']//ul/li/label</t>
+  </si>
+  <si>
+    <t>allCouponsLink</t>
   </si>
 </sst>
 </file>
@@ -498,11 +589,75 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B2802F9-C8EF-4362-B77D-B492C252ABE0}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="45" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -624,123 +779,13 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -749,19 +794,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B2802F9-C8EF-4362-B77D-B492C252ABE0}">
-  <dimension ref="A1:C4"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732602EC-80E6-42FB-9BD0-EB0226F871B8}">
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="2" width="45" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="80.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -777,34 +822,298 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first set of test cases
</commit_message>
<xml_diff>
--- a/FreshGrocer/src/main/resources/TestData/locators.xlsx
+++ b/FreshGrocer/src/main/resources/TestData/locators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJAY\git\Fresh-Grocer\FreshGrocer\src\main\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4485FDD-BB49-4BE9-B742-AAC1C7D9BFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F03C3F-6383-4A70-BAEE-87E3EC21A01F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="83">
   <si>
     <t>locators name</t>
   </si>
@@ -264,6 +264,18 @@
   </si>
   <si>
     <t>allCouponsLink</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'modal-content')]</t>
+  </si>
+  <si>
+    <t>modalContent</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'modal-content')]//button[contains(text(),'Close')]</t>
+  </si>
+  <si>
+    <t>modalContentCloseBtn</t>
   </si>
 </sst>
 </file>
@@ -796,10 +808,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732602EC-80E6-42FB-9BD0-EB0226F871B8}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -998,10 +1010,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
@@ -1009,10 +1021,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
@@ -1020,10 +1032,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
@@ -1031,10 +1043,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
@@ -1042,10 +1054,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
         <v>10</v>
@@ -1053,10 +1065,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C23" t="s">
         <v>10</v>
@@ -1064,10 +1076,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
         <v>10</v>
@@ -1075,10 +1087,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
@@ -1086,21 +1098,21 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C27" t="s">
         <v>10</v>
@@ -1108,12 +1120,34 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>78</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>74</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C30" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>